<commit_message>
3h Battle geht, noch nicht parallel. Auth begonnen
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nahash\source\swen\MonsterTradingCardsGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CDD29E8-6F3C-4B78-8F31-EE1DF47F5196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFAB3585-FD9F-4819-AE08-DC8B137C7A96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1335" yWindow="1305" windowWidth="21600" windowHeight="11385" xr2:uid="{88369686-F968-45CB-887F-E38F2E727DD7}"/>
+    <workbookView xWindow="1365" yWindow="1320" windowWidth="21600" windowHeight="11385" xr2:uid="{88369686-F968-45CB-887F-E38F2E727DD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -625,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D58600B0-3567-4A3D-A785-925E0537D06D}">
   <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="G56" sqref="G56"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,6 +810,9 @@
       <c r="A26" s="6" t="s">
         <v>22</v>
       </c>
+      <c r="B26">
+        <v>3</v>
+      </c>
       <c r="C26" s="6">
         <v>3</v>
       </c>
@@ -970,6 +973,9 @@
       <c r="A51" s="6" t="s">
         <v>41</v>
       </c>
+      <c r="B51">
+        <v>0.5</v>
+      </c>
       <c r="C51" s="6">
         <v>0.5</v>
       </c>
@@ -978,6 +984,9 @@
       <c r="A52" s="6" t="s">
         <v>42</v>
       </c>
+      <c r="B52">
+        <v>0.5</v>
+      </c>
       <c r="C52" s="6">
         <v>0.5</v>
       </c>
@@ -1020,14 +1029,14 @@
       </c>
       <c r="B56" s="2">
         <f>SUM(B9:B54)</f>
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C56" s="6">
         <v>60</v>
       </c>
       <c r="D56" s="2">
         <f t="shared" ref="D56:D58" si="0">C56-B56</f>
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -1052,14 +1061,14 @@
       </c>
       <c r="B58">
         <f>SUM(B21:B53)</f>
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C58">
         <v>52</v>
       </c>
       <c r="D58" s="2">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
3h Lobby works, however 1st thread doesn't get the result
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nahash\source\swen\MonsterTradingCardsGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA46F14-AD5B-4B0A-BF25-617056178075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FDAC9F0-AC77-4C43-9D59-EDB6FE739AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{88369686-F968-45CB-887F-E38F2E727DD7}"/>
   </bookViews>
@@ -625,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D58600B0-3567-4A3D-A785-925E0537D06D}">
   <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,12 +733,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>14</v>
       </c>
@@ -749,12 +749,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>17</v>
       </c>
@@ -764,8 +764,20 @@
       <c r="C21" s="6">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <f>SUM(B21:B26)</f>
+        <v>18</v>
+      </c>
+      <c r="F21">
+        <f>SUM(C21:C26)</f>
+        <v>18</v>
+      </c>
+      <c r="G21">
+        <f>F21-E21</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>18</v>
       </c>
@@ -776,7 +788,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>19</v>
       </c>
@@ -787,7 +799,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>20</v>
       </c>
@@ -798,7 +810,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>21</v>
       </c>
@@ -809,7 +821,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>22</v>
       </c>
@@ -820,14 +832,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B28"/>
       <c r="C28"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>24</v>
       </c>
@@ -837,8 +849,20 @@
       <c r="C29" s="6">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <f>SUM(B29:B34)</f>
+        <v>9</v>
+      </c>
+      <c r="F29">
+        <f>SUM(C29:C34)</f>
+        <v>14</v>
+      </c>
+      <c r="G29">
+        <f>F29-E29</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>25</v>
       </c>
@@ -849,7 +873,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>26</v>
       </c>
@@ -860,7 +884,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>27</v>
       </c>
@@ -898,6 +922,18 @@
       <c r="C36" s="6">
         <v>3</v>
       </c>
+      <c r="E36">
+        <f>SUM(B36)</f>
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <f>SUM(C36)</f>
+        <v>3</v>
+      </c>
+      <c r="G36">
+        <f>F36-E36</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="38" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
@@ -916,6 +952,18 @@
       <c r="C39" s="6">
         <v>2</v>
       </c>
+      <c r="E39">
+        <f>SUM(B39:B42)</f>
+        <v>8</v>
+      </c>
+      <c r="F39">
+        <f>SUM(C39:C42)</f>
+        <v>20</v>
+      </c>
+      <c r="G39">
+        <f>F39-E39</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
@@ -965,6 +1013,18 @@
       </c>
       <c r="C47" s="6">
         <v>1</v>
+      </c>
+      <c r="E47">
+        <f>SUM(B47:B52)</f>
+        <v>1</v>
+      </c>
+      <c r="F47">
+        <f>SUM(C47:C52)</f>
+        <v>5</v>
+      </c>
+      <c r="G47">
+        <f>F47-E47</f>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -1089,6 +1149,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100495F7CC252815B47896F98900E10984C" ma:contentTypeVersion="2" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="afe1b3b164495dc81fdbcdcad6ec8b68">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="207955a2-a3fc-4582-b2ea-e4c7d1fb6048" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b6a42bf87c3f8727d31c248fc1697f6" ns2:_="">
     <xsd:import namespace="207955a2-a3fc-4582-b2ea-e4c7d1fb6048"/>
@@ -1220,22 +1295,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FFD0135-03B1-4A6A-9DC8-B4D791C0671E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="207955a2-a3fc-4582-b2ea-e4c7d1fb6048"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B871BF9-5772-4B74-B6DF-7878EF29873D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0824ED0-660A-437B-A039-7835C5DD208D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1251,28 +1335,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B871BF9-5772-4B74-B6DF-7878EF29873D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FFD0135-03B1-4A6A-9DC8-B4D791C0671E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="207955a2-a3fc-4582-b2ea-e4c7d1fb6048"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
1h General cleanup + improvement: truncate tables
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nahash\source\swen\MonsterTradingCardsGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB231DFA-9569-4E76-82A5-EF63741A4AD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F19CDE16-F2E4-4760-B80C-4E2515F13405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{88369686-F968-45CB-887F-E38F2E727DD7}"/>
+    <workbookView xWindow="-28920" yWindow="2625" windowWidth="29040" windowHeight="15840" xr2:uid="{88369686-F968-45CB-887F-E38F2E727DD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -625,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D58600B0-3567-4A3D-A785-925E0537D06D}">
   <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1152,6 +1152,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100495F7CC252815B47896F98900E10984C" ma:contentTypeVersion="2" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="afe1b3b164495dc81fdbcdcad6ec8b68">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="207955a2-a3fc-4582-b2ea-e4c7d1fb6048" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b6a42bf87c3f8727d31c248fc1697f6" ns2:_="">
     <xsd:import namespace="207955a2-a3fc-4582-b2ea-e4c7d1fb6048"/>
@@ -1283,22 +1298,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FFD0135-03B1-4A6A-9DC8-B4D791C0671E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="207955a2-a3fc-4582-b2ea-e4c7d1fb6048"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B871BF9-5772-4B74-B6DF-7878EF29873D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0824ED0-660A-437B-A039-7835C5DD208D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1314,28 +1338,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B871BF9-5772-4B74-B6DF-7878EF29873D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FFD0135-03B1-4A6A-9DC8-B4D791C0671E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="207955a2-a3fc-4582-b2ea-e4c7d1fb6048"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
30min auth new class, refactoring
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nahash\source\swen\MonsterTradingCardsGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F19CDE16-F2E4-4760-B80C-4E2515F13405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2E1306B-1D31-4CB1-89D5-AB36CECFE3F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="2625" windowWidth="29040" windowHeight="15840" xr2:uid="{88369686-F968-45CB-887F-E38F2E727DD7}"/>
   </bookViews>
@@ -625,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D58600B0-3567-4A3D-A785-925E0537D06D}">
   <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -918,13 +918,15 @@
       <c r="A36" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B36"/>
+      <c r="B36">
+        <v>3</v>
+      </c>
       <c r="C36" s="6">
         <v>3</v>
       </c>
       <c r="E36">
         <f>SUM(B36)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F36">
         <f>SUM(C36)</f>
@@ -932,7 +934,7 @@
       </c>
       <c r="G36">
         <f>F36-E36</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:9" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1114,14 +1116,14 @@
       </c>
       <c r="B56" s="2">
         <f>SUM(B21:B26,B29:B34,B36,B39:B42,B47:B53,B44)</f>
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C56" s="6">
         <v>60</v>
       </c>
       <c r="D56" s="2">
         <f t="shared" ref="D56:D57" si="0">C56-B56</f>
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -1152,21 +1154,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100495F7CC252815B47896F98900E10984C" ma:contentTypeVersion="2" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="afe1b3b164495dc81fdbcdcad6ec8b68">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="207955a2-a3fc-4582-b2ea-e4c7d1fb6048" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b6a42bf87c3f8727d31c248fc1697f6" ns2:_="">
     <xsd:import namespace="207955a2-a3fc-4582-b2ea-e4c7d1fb6048"/>
@@ -1298,31 +1285,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FFD0135-03B1-4A6A-9DC8-B4D791C0671E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="207955a2-a3fc-4582-b2ea-e4c7d1fb6048"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B871BF9-5772-4B74-B6DF-7878EF29873D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0824ED0-660A-437B-A039-7835C5DD208D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1338,4 +1316,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B871BF9-5772-4B74-B6DF-7878EF29873D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FFD0135-03B1-4A6A-9DC8-B4D791C0671E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="207955a2-a3fc-4582-b2ea-e4c7d1fb6048"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>